<commit_message>
Myriad updates to functions and documentation
</commit_message>
<xml_diff>
--- a/inst/extdata/myMeetingsBatch.xlsx
+++ b/inst/extdata/myMeetingsBatch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apk/Desktop/myMeetings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apk/Dropbox/collabCode/zoomGroupStats/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E533EF0-2809-5A45-A913-F7DDA6AA19C5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B3F34B-6605-7A4D-9A40-6A9C30C3F961}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17240" yWindow="500" windowWidth="18500" windowHeight="21900" xr2:uid="{EFCB5279-B430-C249-8837-CDF160FCFA74}"/>
+    <workbookView xWindow="55200" yWindow="1900" windowWidth="18500" windowHeight="21900" xr2:uid="{EFCB5279-B430-C249-8837-CDF160FCFA74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>00000000001</t>
   </si>
@@ -51,16 +51,37 @@
     <t>participants</t>
   </si>
   <si>
-    <t>~/Desktop/myMeetings/meeting001</t>
-  </si>
-  <si>
-    <t>~/Desktop/myMeetings/meeting003</t>
-  </si>
-  <si>
-    <t>~/Desktop/myMeetings/meeting002</t>
-  </si>
-  <si>
     <t>batchMeetingId</t>
+  </si>
+  <si>
+    <t>meeting001</t>
+  </si>
+  <si>
+    <t>meeting002</t>
+  </si>
+  <si>
+    <t>meeting003</t>
+  </si>
+  <si>
+    <t>sessionStartDateTime</t>
+  </si>
+  <si>
+    <t>recordingStartDateTime</t>
+  </si>
+  <si>
+    <t>2020-09-04 15:00:00</t>
+  </si>
+  <si>
+    <t>2020-09-06 15:00:00</t>
+  </si>
+  <si>
+    <t>2020-09-05 15:00:00</t>
+  </si>
+  <si>
+    <t>2020-09-05 15:03:15</t>
+  </si>
+  <si>
+    <t>2020-09-06 15:20:00</t>
   </si>
 </sst>
 </file>
@@ -421,22 +442,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B187BFA2-E9BB-0A49-9D3A-BF37642123E6}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -453,13 +476,19 @@
       <c r="F1" t="s">
         <v>6</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -473,8 +502,14 @@
       <c r="F2">
         <v>0</v>
       </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -493,13 +528,19 @@
       <c r="F3">
         <v>0</v>
       </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -512,6 +553,12 @@
       </c>
       <c r="F4">
         <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switched over from image magick straight to av for the image grabbing. Also changed all video functions to enable user to specify the directory for storing images.
</commit_message>
<xml_diff>
--- a/inst/extdata/myMeetingsBatch.xlsx
+++ b/inst/extdata/myMeetingsBatch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apk/Dropbox/collabCode/zoomGroupStats/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B3F34B-6605-7A4D-9A40-6A9C30C3F961}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAFAA22-6C84-9B46-8F84-060331FC8178}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="55200" yWindow="1900" windowWidth="18500" windowHeight="21900" xr2:uid="{EFCB5279-B430-C249-8837-CDF160FCFA74}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{EFCB5279-B430-C249-8837-CDF160FCFA74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -445,7 +445,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,7 +500,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
@@ -552,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>15</v>

</xml_diff>